<commit_message>
Get daily reddit data: Tue Aug 27 08:09:27 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_01.xlsx
+++ b/data/2024_09_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C479"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,3034 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1f2b192</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>So proud of these 🍉</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22mknfqtq5ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1f2a51d</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>loving the black</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bef3q5ijf5ld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1f2a21r</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Prettiest nails I’ve ever had. 🎀</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/visf32dke5ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1f29shn</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>simple but elegant</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs8sr75eb5ld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1f29elz</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very demure nails 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f29elz</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1f295bq</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Bio sculpture gel to buy</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f295bq/bio_sculpture_gel_to_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1f28rcs</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink coffin 🦋 </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ar0ww4igz4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1f288bb</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Does wearing nail polish help your nails or not?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f288bb/does_wearing_nail_polish_help_your_nails_or_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1f27x8p</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby blue French </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oia3ugenq4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1f27qv9</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Should I go back and ask for re-do?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywb7tcfwo4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1f27qkp</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Love My Toenails, Perfect Color for Autumn😊</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un0stbqpo4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1f27iey</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Modelones Nail Strengthener as base and top coat</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f27iey/modelones_nail_strengthener_as_base_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1f26p28</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm flying high with feathers </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b193gmlue4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1f26hg1</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Can’t go wrong with a classic red</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g27upitxc4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1f263xu</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Do tips make your manicure last longer?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f263xu/do_tips_make_your_manicure_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1f262h1</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>so pretty….?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5qp3hr894ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1f261hn</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>New set made by me . Love it .</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpk8voyz84ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1f25ynh</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The magic nails my friend made me </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f25ynh</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1f25syn</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Do you like them?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f25syn</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1f25rab</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What color is this? </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f25rab</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1f25ea9</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In Love With My Super Duper Stellar Set </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f25ea9</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1f25e51</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Anyone else have to use scraps sometimes? Happy with results considering</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqpyp9tc34ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1f25do2</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>It’s my first time getting nails this long, and typing on the keyboard feels so awkward, but they look so good!</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f25do2</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1f24p3d</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My last summer set for vacation </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f02jeqn7x3ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1f24mwi</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Chrome frenchies for end of summer?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f24mwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1f24m74</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Picnic Mani 🍓🧺🍅</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f24m74</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1f243jr</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Do you guys recommend press on btartboxnails?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f243jr/do_you_guys_recommend_press_on_btartboxnails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1f23xfz</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Rate it please! ❤️</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f23xfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1f23l4g</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>so happy how they turned out!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4iqdh9hqn3ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1f239xv</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>last mani for summer - blue chrome on blue cream w/ contrast double French accents 🩵💙</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyi3qtl4l3ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1f232wk</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby shower nail set </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f232wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1f22j9b</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Nail tech said “Halloween already?”</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f22j9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1f22etq</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Looking for advice and critique x</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f22etq</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1f22b3e</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Nail colors for September?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f22b3e/nail_colors_for_september/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1f22390</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back to school type nails </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oepami3bb3ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1f21fos</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>AoT themed nails!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1ncoxb663ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1f20b0m</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>For my first time I don’t think I did too bad!!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4q5gwr9ex2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1f1zgd8</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Showering with nails</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1zgd8/showering_with_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1f1z5ax</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>coraline inspired nails</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbl4t0yho2ld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1f20zf0</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press-on nails with a unique, super summery design. What do you think? Would you get them done? </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdxb1hoo23ld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1f20n3y</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time ever. Are my cuticles supposed to be bleeding/burning? 💀</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehfd6ud503ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1f20mos</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Very demure very mindful</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upcs5bx103ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1f20fbv</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Light pink this time!</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egc2pd5ey2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1f1y7dg</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Reminder- sometimes it's not you, but products that you use</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugqj50vch2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1f1z22f</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Hey I’m looking for a nude base shade for my French tip?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/riadgufun2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1f1zq4b</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome French tips </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gze0h440t2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1f1zkwb</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Shortie nails in OPI's Dutch Tulips.</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1zkwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1f1zkjg</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday Nails!! </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1zkjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1f1z8sh</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New claws </t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68gq98k8p2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1f1ykqk</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ocean-themed nails 🌊🩵 </t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1ykqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1f1y6ki</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Are these wearable or do they look terrible</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1y6ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1f1xibf</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with my new vitrage work 🤪 how do you rate them? </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1xibf</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1f1xidt</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Romantic Flower Nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1xidt</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1f1xed8</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>i did a nice bright set 💛🌸 before it becomes fall 🍂</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1xed8</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1f1unlt</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+I have done my best to get these results.
+</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8mxnl7fir1ld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1f1wv3b</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>I painted my fav character in the lion king 👑 Medium almonds</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ewmh3p3e72ld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1f1wuwa</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">S’mores moment </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wchajxec72ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1f1wujp</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>I painted my fav character in the lion king 👑 Medium almonds</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zljx4b3a72ld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1f1wn48</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>First time doing freehand french tips</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96jqecpp52ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1f1vrz2</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>I made my own custom waterslide decals at home and I am thrilled with the results! Photos and full detailed tutorial included</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1vrz2/i_made_my_own_custom_waterslide_decals_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1f1w4rv</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Which nail shape looks better</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1241wy322ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1f1w2i9</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time I’ve had my nails done in 6 months </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1w2i9</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1f1vcx4</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>BIAB help!</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1vcx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1f1v2hc</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>I'll never get tired of cat eye polish.</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1v2hc</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1f1uzoy</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>I should’ve color matched her eyes</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1uzoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1f1u3bl</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I prevent brush lines in gel polish? </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1u3bl/how_do_i_prevent_brush_lines_in_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1f1uwsq</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forest fairy nails 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czxlmusjt1ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1f1uelt</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>spiderman themed nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syjik94zp1ld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1f1ubet</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love doing my nails ✨💓 I am just so bad at cutting my cuticles 🥲 any tips? </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1ubet</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1f1rvgn</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Ideas for end of summer nails??</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1rvgn/ideas_for_end_of_summer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1f1i02s</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible to fix this? </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1i02s</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1f1j32g</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>My summer nails inspired by garden beauties and nature colors. What do you think??</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1j32g</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1f1to9l</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>What can i use instead of a cuticle pusher to remove gel x nails??</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1to9l/what_can_i_use_instead_of_a_cuticle_pusher_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1f1tn5u</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>wearing nails even when "looking normal"?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1tn5u/wearing_nails_even_when_looking_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1f1ta3n</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Not sure what to think…</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1ta3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1f1syre</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Idk about y’all, but I’m ready for fall, but still holding on to the last bit of summer with the florals</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1syre</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1f1s9c5</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>new set 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ep8vmoda1ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1f1rugf</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Any way to fix broke nail</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouk6y9ab71ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1f1ro1v</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Are these good? I'm not sure ...</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1ro1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1f1rm7c</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>My set for Halloween!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oif4ce6q51ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1f1rbwf</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s never to early for spooky season. </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1rbwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1f1r4ek</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Lil forget me nots :&gt;</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arubjr9221ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1f1r38h</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Yay we're posting claws now :3 I tried to make these look "natural"</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1r38h</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1f1pdw5</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Acrylic nail shattered off</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1pdw5/acrylic_nail_shattered_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1f1qqzn</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>First time using pressons for free from my aunts small business!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1qqzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1f1pzdu</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Chrome effect at home</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1pzdu/chrome_effect_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1f1qoaw</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>I really like the sharp shape of stilettos, how do you like it?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1qoaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1f1qnzp</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gudetama Nails </t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1qnzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1f1qhc8</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>🥲☠️🪦</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uurjz9jcx0ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1f1qdrq</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>I lost my thumbnail :( what to do in the meantime until it grows back?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1qdrq/i_lost_my_thumbnail_what_to_do_in_the_meantime/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1f1py7x</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>🩵</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6n3750dt0ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1f1pvhw</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These make me want to learn to figure skate </t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1pvhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1f1pevk</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Beach galaxy mashup - my favorite set EVER 💜💙</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ytzj9wcp0ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1f1or44</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Pink chrome and heart shaped cherries 💗</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1or44</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1f1o07x</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don't care that it's still summer it's PSL nails time </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1o07x</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1f1nzi2</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>I just felt Sukuna’s presence… What the hell is happening in Shibuya!?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1nzi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1f1ny46</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Prep before applying new layer or topcoat?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f1ny46/prep_before_applying_new_layer_or_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1f1ntnw</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>This white set is so simple and cute!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1z83qftfc0ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1f1mwpw</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Staining on finger nails?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ve2ah6p40ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1f1mlla</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Gel Nail Extensions for the first time ✨</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dv3m5as10ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1f2bjli</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Fall skittle</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2bjli</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1f286yj</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else out here rocking the chaos of different lengths and shapes AND colors for each nail? </t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmbvvr7at4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1f27tdv</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Finally found the best way to wear this sheer flakie I had half a mind to destash, now I love it (In the garden mystery flakie, Kathleen and co)</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qz2lrdclp4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1f27cf9</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Dream Formula</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmrjftywk4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1f2799z</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>The colors remind me of cotton candy!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2799z</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1f26jmy</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Can’t go wrong with a classic red ❤️</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ur3o8kdhd4ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1f26blk</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bloody and Bruised! </t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f26blk</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1f2686m</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible for an acrylate allergy to only impact my ears? </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f2686m/is_it_possible_for_an_acrylate_allergy_to_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1f262jn</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My sister cleaned out her closet… </t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5xnw9j994ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1f25cob</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Was going for spoopy purple and ended up with ~grapes~</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f25cob</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1f255x8</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>My first PPU order came today!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90r3ulbb14ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1f25375</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No Longer Human cover inspired nails! </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f25375</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1f24eht</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Holo Taco: "The Floor Is Guava" and "Electric Sweetener"</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv7b3aoju3ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1f246x0</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Cursed Glitter Skittle (and one gradient)</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f246x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1f2441b</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A good blue glitter is my true love </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojmsjj75s3ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1f23xyp</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>how do I get started learning how to do nails?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f23xyp/how_do_i_get_started_learning_how_to_do_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1f23bxi</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>French mani base polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f23bxi/french_mani_base_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1f22x2d</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP- wide brush replacements? </t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f22x2d/ilnp_wide_brush_replacements/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1f22mz2</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Zombie Queen 🧟‍♀️💚🐍</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f22mz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1f22b9f</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just try doing the thing. </t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f22b9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1f21vek</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want my nails to look like they’ve been kissed by a biblically accurate angel. </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f21vek</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1f21v7h</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Yes, but we haven't had second breakfast.</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmces8vh93ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1f21hg0</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Lemming Laquer - Dead to the World</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f21hg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1f21dwf</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>My first time breaking a bottle of nail polish since I was a kid. RIP Holo Taco’s Lemon Sucker. 😭🪦</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f21dwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1f20ao3</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>My first magnetic!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6khmjr5bx2ld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1f1yz00</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Did my nail tech miss the mark on the magnetic nails I asked?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1yz00</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1f1yqax</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>The Skunk Who Saved Books....</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1yqax</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1f1ykq8</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>I can't get anything to stick</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1ykq8/i_cant_get_anything_to_stick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1f1yfz6</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>It’s PSL season 🎃</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p2zkc46j2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1f1xmmh</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>How I’m feeling…</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1xmmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1f1x2vf</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>My nails finally stopped peeling</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1x2vf/my_nails_finally_stopped_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1f1w783</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>I've gone through half the bottle of Mallcrawler already lol</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y0pmc6l22ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1f1v3ie</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>we never lie about bunnies, bunny 🐇</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1v3ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1f1v2lp</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Top Coat advice</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1v2lp/top_coat_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1f1uwkg</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Realized my nails match my Bluetooth speaker 💅</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfcm375it1ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1f1unad</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Sealing the free edge</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1unad/sealing_the_free_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1f1ugxa</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I prevent brush lines in gel polish? </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1ugxa/how_do_i_prevent_brush_lines_in_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1f1ufqr</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>A lil neon, a lil sparkle</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aco7hso6q1ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1f1uagm</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>ILNP Vineyard Collection swatches [PR]🍷</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y63qfsr3p1ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1f1t71w</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Loving this layered look!</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1t71w</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1f1sv00</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Acrylate free nail glue</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1sv00/acrylate_free_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1f1revq</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sending nudes </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1revq</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1f1rbsx</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Morpho Glow dupes?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oug5jznl31ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1f1r9fe</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>ILNP - Flashing Lights</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1r9fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1f1r0dy</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>This is dumb but I love it - top coat shrinkage solution</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1r0dy/this_is_dumb_but_i_love_it_top_coat_shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1f1qt64</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Second time this week 😭</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1qt64</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1f1qmic</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Is it possible to develop an allergy to non-gel polish?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1qmic/is_it_possible_to_develop_an_allergy_to_nongel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1f1otwl</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can a total glitter bomb and a flashy linear holo still feel so dainty? </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1otwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1f1oqte</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>my nails r constantly breaking and tearing from working in a kitchen what do i do to make them stop breaking</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1oqte/my_nails_r_constantly_breaking_and_tearing_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1f1od0z</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Elden Beast </t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14lft996h0ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1f1nc0d</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Nails ... in ... Spaaace</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1nc0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1f1n0ep</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little neon to close out summer </t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbjxlm8m50ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1f1lrb1</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunshine ☀️ </t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqbac8ijtzkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1f1lge7</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday Mani! 🎂 </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05bvfkraqzkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1f1ld64</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I cannot stop staring at my nails  </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/56s78ggfpzkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1f1khdo</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1khdo/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1f1k58q</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Horseshoe magnet for magnetics ?? </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1k58q/horseshoe_magnet_for_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1f1jdyx</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Crackle topper tips? </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f1jdyx/crackle_topper_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1f1j22a</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dabbling in Clone Research by Swamp Gloss </t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7v0i0lccxykd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1f2b6og</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>A manicure I got before that I was very satisfied with, it looked great!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oaqdbf4to5ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1f2at4k</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Yogurtnail top gel</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f2at4k/yogurtnail_top_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1f2ap83</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking delicious 🤤 </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ackqpt1mm5ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1f29r7q</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>🍒🌺🍷</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mntf6dbza5ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1f25ehb</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Compared to my first try I think I’ve improved with my self teachings💕</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f25ehb</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1f22sae</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Need Ideas</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f22sae/need_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1f20ggj</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>A little extra protection for the week 🧿</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqy801rny2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1f1z9og</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glow in the dark! </t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3ab5x2fp2ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1f1yt1u</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>I attempted to make DIY waterslide decals and I am OBSESSED with the results. Here’s a full tutorial!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f1yt1u/i_attempted_to_make_diy_waterslide_decals_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1f1wx9a</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>I painted my fav character in the lion king 👑 Medium almonds</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kjogyhjt72ld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1f1uy4p</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bejeweled nails </t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1uy4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1f1ux7d</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forest fairy nails 🧚🏿 </t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0n7wgtmt1ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1f1rmqe</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My set for Halloween </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4lwk36u51ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1f1rdlr</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">August nails </t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jkv1p0z31ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1f1rddv</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Help with using chrome powder on designs</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1rddv</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1f1qj9i</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding in 2 weeks and need to decide my nails! Dress and inspo in the post. </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f1qj9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1f1ooep</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mix and match 🌊 </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0em4o1qj0ld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1f1lyrt</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Got to make these the other day :)</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xx3vyscnvzkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1f1l80o</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eyes on the prize </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5byc0cmsnzkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Aug 28 08:09:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_01.xlsx
+++ b/data/2024_09_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C479"/>
+  <dimension ref="A1:C638"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8579,6 +8579,2709 @@
         </is>
       </c>
     </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1f34ad7</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ocean/beach/summer nails before summer ends </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f34ad7</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1f33i3o</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Is there an app for nail designs?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f33i3o/is_there_an_app_for_nail_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1f32y3y</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Summer colors before summer ends sigh</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f32y3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1f32vhu</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail prices. Pedi &amp; mani, both gel.    $90 today </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f32vhu/nail_prices_pedi_mani_both_gel_90_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1f32rhs</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>They asked me for them for a party.</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f32rhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1f326c5</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Press On nails puss into cuticles?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f326c5/press_on_nails_puss_into_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1f31yjr</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing nails! </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f31yjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1f31rs8</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>so proud of myself for this set 💞</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lv1i9mo4cld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1f31na1</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Seems there is no copyright in nail art industry</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f31na1/seems_there_is_no_copyright_in_nail_art_industry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1f30xop</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set, or can they just trim them? </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpv0lvc1wbld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1f2zvev</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best way to remove polish without remover? </t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2zvev/best_way_to_remove_polish_without_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1f2zqfn</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>How are my new nails?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5ig4vs8kbld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1f2zksi</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essiexwicked but pink/ purple base? </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2zksi/essiexwicked_but_pink_purple_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1f2zg16</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>what nail shape for me? my nail beds are so tiny and my hands are short and stubby</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efjqmvdjhbld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1f2z6dq</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>I’m learning…</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2a576z3fbld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1f2yh0u</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer Squiggles </t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9scuyhu8bld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1f2xgb9</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice 🪲 </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2xgb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1f2x3qh</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Hard gel newbie</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2x3qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1f2wuam</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>morning tea. 💜💕☕️✨</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oelsfzjouald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1f2wjrz</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Pink Cat Eyes! 💓</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2wjrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1f2wfd3</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>How much do you give my manicure from 1 to 10?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mun6kmy2rald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1f2w87c</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>My claws!!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wai361hgpald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1f2vz5q</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>What’s the best acrylics for a first timer ?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2vz5q/whats_the_best_acrylics_for_a_first_timer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1f2vpqk</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Press-ons &amp; oil</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfbswt68lald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1f2v972</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lily and fox nail wraps with a top coat </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70cciu4ihald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1f2uwkf</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Can you rate my nails?💖They are my first ever(im trans)🎀</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2uwkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1f2uveg</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friend is a nail tech now! She did these for me </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qlzmzljeald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1f2u2b5</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Nails </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6m15a168ald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1f2u1y2</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>£50 and in love. Totally worth it</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2u1y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1f2tso8</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute little freehand design </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty3fepv56ald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1f2qyd2</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Advice for a guy wearing nail polish at work</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2qyd2/advice_for_a_guy_wearing_nail_polish_at_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1f2tmcd</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My bridal shower nails! I’m obsessed </t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2tmcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1f2t8zs</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Loving my new snake nails</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2t8zs</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1f2swbd</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New press on set I made! Maychao Tips + Modelones 1636 </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxz9wgehz9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1f2shsg</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple line art </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2shsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1f2rz7b</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to stop my pinky nails from growing like spoons? </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20cbbiejs9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1f2rxlt</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Powerpuff Girl Nails</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2rxlt</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1f2rp2h</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>What do you think about my new design?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2rp2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1f2r3qz</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Cherry Bomb 🍒🇫🇷</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww2xlb10m9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1f2r22y</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Paid 102$ for these, tip is added into that... Worth it or nah?...</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2r22y</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1f2qn7o</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Gel extensions. Do you like them?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg2oddami9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1f2qczr</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Help: Gel Polish</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2qczr</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1f2q4z2</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>What’s the best nail shape for me?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akv3ra0ye9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1f2pzo5</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Sea foam gelish</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad43hclud9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1f2o8z6</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>coraline themed set 🪡⭐️</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkxh818g19ld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1f2nxkv</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Glitter! 😍</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh7roc57z8ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1f2nwpe</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Unsanitary Tools</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2nwpe/unsanitary_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1f2ns72</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>🍒❤️</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2ns72</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1f2nnlg</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Loving my nails! I did it myself!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2nnlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1f2ngyh</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2ngyh/nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1f2n2bw</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Did my own nails today</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2n2bw</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1f2mb2d</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>is it a delicate design?💙</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbkptq1hn8ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1f2ma3g</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i did my first ever set of gel extensions, what do you guys think </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2ma3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1f2m8wa</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>So these look right?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2m8wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1f2lm5c</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>My toe nail keeps breaking and I need advice. (CW: feet)</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nejsecmi8ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1f2l25i</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Natural nail love</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2l25i</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1f2l8t3</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Red ♥️🍒</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2l8t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1f2l4gj</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think about my nails 💅 </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqxd0ugze8ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1f2kz6a</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Did my nana's nails!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0r7j77wd8ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1f2555f</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Tips for the Interim?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2555f</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1f2kww0</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Would it be weird if I get my nail lady a card?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2kww0/would_it_be_weird_if_i_get_my_nail_lady_a_card/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1f26162</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>What words do I say to get my nail tech to recreate a look like this? Inspo pics from The Gray Details, NailswithAby, and Cassidy Brotherton</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f26162</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1f2i8im</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>My favorite set ✨👼☁️✨</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2i8im</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1f2imoz</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Barbie Girl Birthday Set</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2imoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1f2j69b</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Lisa Frank Nails</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2j69b</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1f2jtyw</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>What would you call this nail shape?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2jtyw/what_would_you_call_this_nail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1f2kah2</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>I think I found a color that looks okay on my hyper-pigmented hands</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2kah2</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1f2kgs6</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>What color should I have done?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2kgs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1f2k0ub</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Newest set - Classic French with gold sparkles ✨</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3wj2ast68ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1f2jvtj</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Crispy wedding set </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jg6e2zs58ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1f2jiaa</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help , my nails got damaged </t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2jiaa/help_my_nails_got_damaged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1f2j3x2</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Early fall flower set</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2j3x2</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1f2j19t</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Summer shells 🐚</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7mubhdoz7ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1f2iy5l</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>🥰</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2iy5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1f2ixts</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So proud of this application </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2ixts</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1f2iqjv</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ll be 36 this Thursday but I will never be too old for glitter! </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g31y3uix7ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1f2ilvx</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>What's the best top coat? Need recommendations as My bottle is almost out and I do not really want this again. 💅</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn2ikx6lw7ld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1f2il1k</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i'm in love with this </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn5uhww7w7ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1f2hc9s</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>beautiful cherry design 🍒</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffwfs5yym7ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1f2h89i</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone know how to stop dee hangnails? They only happen on my thumbs! </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncburiw0m7ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1f2gyxe</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Sharp Stiletto Advice Needed</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1xlr25wj7ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1f2gyqi</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Did i eat or nah (my first set)</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2gyqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1f2gmva</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>I base my personality on my nails</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c85zx2b6h7ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1f2e8fx</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I was looking for something unique yet simple, so I chose a purple gradi</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2e8fx</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1f2e1je</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Timeless classic🩷</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ks52nrfws6ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1f2dmzp</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherries 🍒 </t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2dmzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1f2cxmj</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best nail shape for short nail beds? </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2cxmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1f2cpiq</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red French tips </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2cpiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1f2c26o</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flowers 💐 </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7ffn4fh46ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1f2c22w</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got some cheap press ons from Amazon. Still trying to figure out the sizing but I think I did a good job so far. Color is OPI chopstix and stones. </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2c22w</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1f32x8h</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Mani refresh question</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f32x8h/mani_refresh_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1f32vtr</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>I thought this was polish</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br6z2sijhcld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1f31uyb</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>impatiently waiting for autumn 🎃</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekvgyotn5cld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1f31qxq</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Jelly help?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f31qxq/jelly_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1f31p5b</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Which Seche Vite top coat to get?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f31p5b/which_seche_vite_top_coat_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1f30b2a</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Needed to show someone 🌈</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/get1492spbld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1f30ayk</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sally Hansen x Despicable Me 4 </t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f30ayk</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1f2zx6c</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Shimmer toppers that give a similar effect to these polishes? </t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2zx6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1f2yst2</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for recommendations </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2yst2</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1f2ypib</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Blue skittle 💙🩵</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2ypib</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1f2ypa7</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Modern version? </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2ypa7</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1f2xwlb</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Similar to ILNP Eclipse/KB Shimmer Obsidian but more blacky/red?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f2xwlb/similar_to_ilnp_eclipsekb_shimmer_obsidian_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1f2xvqw</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>my birthday nails!! nails to match my dress:)</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2xvqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1f2x5i0</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Dupe?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxgj5jadxald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1f2wq3x</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Dupe for Chanel Pink Tonic? Not my pic obvs!</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rwd1himtald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1f2wmme</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Pink Cat Eyes! 💓</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2wmme</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1f2vw1f</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Comparison request</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f2vw1f/comparison_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1f2v8m8</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - two shades 🩷💚</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2v8m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1f2urzl</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s time for a monthly mani roundup! </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2urzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1f2u8s1</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Sassy Cats - “The Right Catitude” (HHC 07/24) &amp; “Double Love” (PPU 08/24)</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rogov8kk9ald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1f2u4n6</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce, Read between my tulips </t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2u4n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1f2u49i</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>How long do Cirque's limited collections usually last?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f2u49i/how_long_do_cirques_limited_collections_usually/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1f2tqir</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Essie Gel Couture Top Coat work with other polishes?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f2tqir/essie_gel_couture_top_coat_work_with_other/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1f2tgnk</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black? Red? Both? Both! </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2tgnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1f2tdkk</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>First thermal!</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2tdkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1f2sr3a</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>ILNP Campground Crèmes [PR]</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2sr3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1f2sn31</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Mourning nails</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f2sn31/mourning_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1f2sjke</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moon at collection finally arrived!! </t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2sjke</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1f2s1f4</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>🧛🏻‍♀️🦷Orbite Me🦷🧛🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uive4jozs9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1f2qsu0</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>I found the limit to my skills and I'm dying</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2qsu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1f2qeqg</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>ethereal glam ✨</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upcyh9cwg9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1f2prql</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>For this weeks mani: Classic Red</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2prql</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1f2po6c</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Matchy matchy</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2po6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1f2pk1s</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Holo Taco and Lights Lacquer?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2pk1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1f2phd0</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Scream Nails haul!! And SALE! </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsacuh75a9ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1f2ofa9</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>ORLY’s thermal glitter topper, Bring The Heat</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk2rcuno29ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1f2nzs3</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Difficult formula but suuuuuch a pretty color!!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2nzs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1f2n4kz</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Learning from Redditors</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2n4kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1f2msuc</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Is it Autumn yet?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fswse1n0r8ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1f2lyli</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fairy dust 🧚‍♂️ </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2lyli</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1f2lump</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Little foxes 🥰</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2lump</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1f2lkv9</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>🐟🪷Koi Pond🪷🐟</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2lkv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1f2lglr</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Matte Battle of the Boxes 💚🖤🩵</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2lglr</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1f2knc0</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Before I reorganize all swatches…</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2knc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1f2jsr7</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Looking for a gel to match this</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdbgpaw658ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1f2jrn0</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Cherry Nails</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2jrn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1f2jplk</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>amid the insects’ lulling serenade 🪲</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2jplk</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1f2jj3l</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>First time buying a holo polish, definitely not going to be the last 🤩🤩</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wxykxgm638ld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1f2i62h</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>First thermal, pictures don't do it justice</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2i62h</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1f2hulo</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Totally Gobsmacked, Indeed</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p9yix9vuq7ld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1f2h833</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Fun with a dark, smokey blue creme 🙃</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/GHoqMiS</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1f2fll4</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Essie Smooth-e missing from shelves?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f2fll4/essie_smoothe_missing_from_shelves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1f2fi4o</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Watermelon or strawberry banana 😍😍</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2fi4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1f2d4zz</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So we’re going full PSL I see… </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2d4zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1f2bzt3</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>I hate Essie.</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f2bzt3/i_hate_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1f34qim</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>One of my favourite sets ❤️‍🔥😍</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzk92gvr4dld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1f33m3z</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Is it delicate?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pnf0f4cqcld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1f339ua</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A rookie attempt~ </t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/km9pspb3mcld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1f31vio</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Beetlejuice 🪲…, Beetlejuice 🪲…,</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f31vio</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1f2ziw0</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uiat7n9ibld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1f2y5vg</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>A nude base with rhinestones, thank you to my nail artist Kimmy! I love it!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu77gy455bld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1f2xgop</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice 🪲 </t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2xgop</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1f2vzz7</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pokémon nails! </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/or3eeszjnald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1f2si6l</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stamping advice </t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f2si6l/stamping_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1f2k1fn</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Barbie style 💕</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zan9n1by68ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1f2ir33</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">witch nails </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2ir33</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1f2g4vk</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Blue or green?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7l7oopd0d7ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1f2czvf</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Sea nail design</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3026u5qqg6ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1f2cwfy</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunset Ombré </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9ixzb8if6ld1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Aug 29 08:10:01 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_01.xlsx
+++ b/data/2024_09_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C638"/>
+  <dimension ref="A1:C803"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11282,6 +11282,2811 @@
         </is>
       </c>
     </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1f3v8hp</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you guys use Pinterest for buying nails ? </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3v8hp/do_you_guys_use_pinterest_for_buying_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1f3tmfu</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Finding a Nail Tech</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3tmfu/finding_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1f3rsp2</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>DIY Thermal French 🌸</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3rsp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1f3vkka</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Green Cat Eye</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/em8c22bjqjld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1f3vdlk</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>after biting my nails for 10+ years… my first two gel sets to try quitting</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3vdlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1f3udrz</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Surgery nails ?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3udrz/surgery_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1f3tbv7</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>extension got caught and real nail ripped off, what do i do?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3tbv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1f3u6xs</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Is this nail colour too pale for my skin tone? Unsure..</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3u6xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1f3td1o</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Blue marbles</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75trbr6d1jld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1f3t12u</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it worth starting a press on nail business? </t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3t12u/is_it_worth_starting_a_press_on_nail_business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1f3so57</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with my last set </t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5omjsupiuild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1f3si6w</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Mosaic French</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3si6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1f3sdrr</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding Nails </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8s5ojvyqrild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1f3sah7</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Reusable Press-Ons?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3sah7/reusable_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1f3rsgn</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Nail tech gave me my perfect first set!</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3rsgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1f3rqk2</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Nails by: nayelinaildit</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3rqk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1f3rj20</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>This might be my favorite set yet 🐚🤍</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbrba494kild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1f3r7vw</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t xml:space="preserve">vet tech nails </t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3r7vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1f3r7to</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>My delicate nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hqbjn3ehild1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1f3qyzs</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>I have a feeling that l'm going to get proposed to soon. What would you recommend I do for my nails?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3qyzs/i_have_a_feeling_that_lm_going_to_get_proposed_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1f3qvjm</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Love my jelly extension nails, especially when they are under the sun❤️🥰</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9291bv0eild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1f3qsvp</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cottage nails for my upcoming trip to the highlands </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3n3zhguudild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1f3qqdn</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Loooooooong time lurker but I couldn’t lurk anymore lol</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/py24xs29dild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1f3qm51</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Pretty Ombre to match my keyboard</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3qm51</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1f3q4x4</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of Autumn 🍂 </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3q4x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1f3pyov</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Beginner advice</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3pyov/beginner_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1f3pc6v</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I do color or clear polish? </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3pc6v/should_i_do_color_or_clear_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1f3phiq</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Peachy Chrome to compliment my new ring 💍💒</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9c6h6u2i2ild1</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1f3pful</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>My growth 😭</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dkdcxm32ild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1f3p49y</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tragedy struck today :( </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fajevhczhld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1f3owji</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Natural nails with builder gel</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3owji</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1f3ool5</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Almond or square?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3ool5</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1f3oc5d</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Butterfly nails from me to myself 🦋</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxrr6awmshld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1f3o7lq</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Fall nails ft. Mr. Pickles 🍁🍂🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fkc12elrhld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1f3o580</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Milky white almond </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3o580</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1f3eqtn</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Question re: fake nails</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgqmpyysmfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1f3f3bl</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you use builder gel like normal gel like just paint it on? </t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3f3bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1f3g6ic</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>execution vs inspo</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3g6ic</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1f3l1bh</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Why are some of my hard gel mani nails having this dull/ matte effect on part of the nail?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmo3cm8s3hld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1f3nuap</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Feelin’ blue</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq6sawvkohld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1f3jyrp</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Base coat with collagen</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3jyrp/base_coat_with_collagen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1f3nybu</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Pixar Nailart 🥰</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0wkxkngphld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1f3nojm</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Got them browny today</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esqvirr5nhld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1f3n4pf</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using soft gel extensions </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cesw2oh0jhld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1f3n1vs</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>My first attempt at jelly fruit nails!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3n1vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1f3mvf8</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Can’t help but overdecorate 🎀</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dwfj022hhld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1f3mhoh</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Wet N Wild- Disturbia</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3mhoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1f3lv87</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Is builder gel a good option for thing bendy nails?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3lv87/is_builder_gel_a_good_option_for_thing_bendy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1f3lsfh</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Sig color</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yi88v3s49hld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1f3lo8t</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how cute </t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqxjfg8b8hld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1f3ljj5</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>🩶 ILNP Tombstone 🪦</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3ljj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1f3ljef</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Galaxy colors</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2hxl0nc7hld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1f3kx04</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>My favorite end of summer manicure before the fall</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3kx04</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1f3kwks</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Soot sprites!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qf7rcqv2hld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1f3kt9t</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Flirty nails</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6lne7p82hld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1f3kszb</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Dragon egg nails</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kp38qff62hld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1f3krsh</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creating a beetlejuice nail set 🥰 here is the Sandworm 🫢💞 yes these are 10 XL sizes 😆🙌🏼 can't wait for the rest </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oaxqrpex1hld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1f3jrk4</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nails, a beauty that I love... With chain, pendant, mirror effect... and many details </t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1e6dg3mhngld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1f3jnff</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>They aren’t perfect but I’m so proud that I did these! My favourite set so far.</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ry0ao2mmgld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1f3jk1h</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>The nails of a silversmith! 2 long, 3 short</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr3s5rgwlgld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1f3gxsq</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>What do I need to start doing gel polish at home?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3gxsq/what_do_i_need_to_start_doing_gel_polish_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1f3izq6</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Help me find a color!</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xto3qlshgld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1f3ht21</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Best nail product for working hands?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3ht21</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1f3i8mc</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Work Nails</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxm29uh5cgld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1f3i7d5</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Airbrush ombré </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5o0cuklvbgld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1f3hw7o</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yellow nails </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3hw7o/yellow_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1f3h8sf</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Charmed out lol</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5iyuudx4gld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1f3gjyt</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Natural nails and Brazilian manicure, I love this blue nail polish</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3gjyt/natural_nails_and_brazilian_manicure_i_love_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1f3gjoa</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Took your advice from my last post, tried to reshape them myself</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3gjoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1f3gjke</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Half cover nails + builder gel?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3gjke/half_cover_nails_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1f3gip0</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Home Gel Nails??</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3gip0/home_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1f3ge5r</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Totally obsessed with my new nail color!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3ge5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1f3gbv9</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>How is this effect achieved??</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18mmbsxayfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1f3fzb5</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Nohing like an ice cold beer after a long day at work! How do y'all spend your evenings? 🥰</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsio1xcevfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1f3fsyj</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>How I love blooming gel</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dezhtr2hufld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1f3fkuz</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Nails I did for my sister ☺️</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9wrc7uusfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1f3fcfy</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Heartbreak 💔</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35bcgse8rfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1f379po</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Question about gel application</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytxz9yyazdld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1f2v3w7</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Why is my apres gel extension + gel polish see through?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejb2bj4dgald1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1f2vem0</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>4th DIY GelX Set</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2vem0</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1f2weh5</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Got nail extensions and acrylic overlay to help grow out nails. Ring of fire damage.</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2weh5/got_nail_extensions_and_acrylic_overlay_to_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1f2wgzp</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Are my nails too thick</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2wgzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1f2wloc</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>French manicure with added tips</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2wloc</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1f2ysi7</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>How do you remove curry stains off a regular manicure?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2ysi7/how_do_you_remove_curry_stains_off_a_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1f2z46h</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dip powder </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f2z46h/dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1f2zxfa</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Nail Reformation Press ons?!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f2zxfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1f307jr</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>air bubbles on nails?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asdo630tobld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1f31vea</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>First time getting tips &amp; acrylic.. is this good or bad?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cqzghsbs5cld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1f3acwy</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>tamagotchi inspired nails!! :3</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3acwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1f3emz1</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommended product List Beginner </t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3emz1/recommended_product_list_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1f38izx</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hair dye vs nails </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f38izx/hair_dye_vs_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1f3bz0h</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time gel? </t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j38qw2cv2fld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1f3dc8o</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>I Choose You by Glam Polish</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ek2gdkprcfld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1f3an99</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Press on nails that fit like Olive &amp; June</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f3an99/press_on_nails_that_fit_like_olive_june/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1f3bknh</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>New to gel, nail underlayer cracked?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3bknh</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1f3d5ph</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suggestions </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bxf648fbfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1f3eb4c</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>I think I’m a square girly now….</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nljm60knjfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1f3e2j1</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Nail Sticker. So far i love them.</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8zi958yhfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1f3dtmm</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Halloween nails (press ons from Walmart)</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh5y3zd8gfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1f3dssp</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abstract nails (: </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3dssp</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1f3vdzn</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Help me find the perfect mauvey brown!!</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3vdzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1f3u94x</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Dance legend polish</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulee42dwajld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1f3stec</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Ethereal Pigeon</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ep6bjhlwvild1</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1f3sdzc</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Sally Hansen Heart of Sass</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ow5vly2srild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1f3rw50</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Minimalist Spotted </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdfrjeidnild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1f3rc8x</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>iridescent baby blue 🩵</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9jhqqpgiild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1f3qrrj</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>thermal french tip</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3qrrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1f3qq0x</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Lurid’s shimmers are my favorite ✨</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3qq0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1f3qlu2</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which cart would you check out? </t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3qlu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1f3p2ye</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>My fiancé suggested forest 🌳 vibes 💅</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgn48hu0zhld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1f3oy46</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Best finish/polish for indoor lighting?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f3oy46/best_finishpolish_for_indoor_lighting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1f3nf6z</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Little Serpent</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xz79iol9lhld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1f3ndp2</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>What are some of the rudest comments you’ve heard regarding your manicure?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f3ndp2/what_are_some_of_the_rudest_comments_youve_heard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1f3n4rm</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PSA - KBShimmer Clearly on Top and HT Magnetics </t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5csnj01jhld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1f3mx0y</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t xml:space="preserve">have you guys seen this? </t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/st1diev81hld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1f3mv58</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Searching for a similar color</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bg5feqd0hhld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1f3liw4</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>🩶 ILNP Tombstone 🪦</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3liw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1f3lf58</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>It's giving "90s mom lipstick" ...</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3lf58</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1f3l7df</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Thin nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3l7df</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1f3l5u7</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Follow Your Dreams</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.imgur.com/a/m6HiQSk</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1f3l0sj</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Emily de Molly replacement brush: does it fit in Cirque bottles?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3l0sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1f3k11u</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lyn B - Am I just paranoid of Emma stone? </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3k11u</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1f3jzrg</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Snowhere Else I’d Rather Be</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q85yq94nwgld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1f3jo1h</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce - First purchase! In love with Cock-a-doodle-Doom + Fierce Mojo (accent nails)!! </t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wi7n6evomgld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1f3ja72</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Not bad for £3 - I'm usually not a fan of blues!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3ja72</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1f3j1is</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Hazy lavender flakes 🪻🌫️</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3j1is</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1f3iz0v</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Favorite light pearl/opal polishes? No gel/powder</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f3iz0v/favorite_light_pearlopal_polishes_no_gelpowder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1f3ipu9</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Lurid Laquer is so glowy!</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5h526mofgld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1f3inhv</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I HATE Lights Lacquer </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f3inhv/i_hate_lights_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1f3iasz</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>It’s fall!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3iasz</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1f3i5z6</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Aquarius Water Marble</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3i5z6</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1f3hlyv</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>i was asked to try incorporating real sand into my nails…</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1vpkz3kk7gld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1f3hi22</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>ILNP Annabelle</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3hi22</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1f3h5nk</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are some good non traditional fall colors? </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f3h5nk/what_are_some_good_non_traditional_fall_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1f3fxy8</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Differences between BKL The Asteri and 2.0?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f3fxy8/differences_between_bkl_the_asteri_and_20/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1f3exeh</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Tropic Low </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3exeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1f3e6dw</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Fall isn't coming soon enough!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htpfpfgoifld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1f3ckog</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>S-s-silver~</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66jahac87fld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1f3c2t8</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails matching my hair </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3c2t8</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1f3bwa7</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Death Valley Nails stock?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f3bwa7/death_valley_nails_stock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1f3bjql</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I didn't have a 30 lb horseshoe magnet, but I did have a 1200 lb magnet </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3bjql</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1f3aqpm</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Today's nails.</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxin5kvvteld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1f39fx4</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Which polish would you go for with this skin tone?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqp4ggjljeld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1f38kbp</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>3 coats, careful application, still have a bald spot. Any way to prevent this or just keep applying?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypdpq8cubeld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1f38cgp</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Your favorite sun-bleached shades? </t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxnvu9cx9eld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1f386b2</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Vineyard 🍷 </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f386b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1f37izi</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glass Jellyfish 🪼 </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f37izi</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1f35yfr</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>BKL - Goddess of Rot</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f35yfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1f3wjbt</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwztq24v2kld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1f3tf7f</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Mosaic French</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3tf7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1f3t99s</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Spooky season is here!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/in58j5ab0jld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1f3r5ap</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lavender spider 🕷️ </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djb278brgild1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1f3kxc3</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Last summer set 🍒</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3kxc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1f3kqyq</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creating a beetlejuice nail set 🥰 here is the Sandworm 🫢💞 yes these are 10 XL sizes 😆🙌🏼 can't wait for the rest </t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5tol4z8s1hld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1f3jmu7</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pixar nails </t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvp1n0ihmgld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1f3hkmz</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>💜✨ Opi Pompeii purple ft. Essie special effects ethereal escape ✨💜</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3hkmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1f3gga1</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Casual set</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acrdhvx5zfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1f3fw85</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Shark week nails</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3fw85</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1f3fv93</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Teal and orange moment</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3fv93</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1f3ftcy</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>A little retro moment</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3ftcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1f3fede</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Tequila and lime</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3fede</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1f3e8gt</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Why does my nail polish sticks ?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f3e8gt/why_does_my_nail_polish_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1f3dggv</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Love these</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1hp0vwldfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1f3dd98</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Freestyle Jelly Color Set with The Nails Bae Gold Chrome. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohhm7hbzcfld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1f39wkl</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m obsessed </t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ho3daxjcneld1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Aug 30 08:10:00 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_01.xlsx
+++ b/data/2024_09_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C803"/>
+  <dimension ref="A1:C976"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14087,6 +14087,2947 @@
         </is>
       </c>
     </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1f4phe1</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>First set since moving!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4phe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1f4orxt</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Very cutesy, very demure🪽</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4orxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1f4ok97</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>3d Green set💚💚</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4ok97</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1f4oi3d</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>New whimsy set</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4oi3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1f4oew9</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Alien nails 👽😍💖</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51qr9x8tvqld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1f4o75l</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would it look dumb to do all my nails but one? </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f4o75l/would_it_look_dumb_to_do_all_my_nails_but_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1f4no4l</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>✨🖤</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2sb3jmumqld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1f4nmwg</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Spooky season 👻</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4nmwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1f4mt4l</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Ending the summer with a bang 💚</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/901ywofbdqld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1f4msia</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>my new nails that I love</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kreilnu4dqld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1f4m4pf</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>In my stiletto era</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxnn3zw96qld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1f4lwb8</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with this blue! </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/856h7hjx3qld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1f4lr9a</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Male in need of nail advice</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f4lr9a/male_in_need_of_nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1f4lprj</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>At home Polygel practice</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs6auzx32qld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1f4ln0t</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first set in a minute. very happy with them! </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qol1yjyb1qld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1f4lc8n</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time ever doing my nails, I need help </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4lc8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1f4kolc</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4kolc</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1f4e0ve</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Cracked nail - keep it together?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4e0ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1f4gui4</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling out of inspiration lately. But still managed to squeeze these out after 3 restarts. </t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0i8suh5uold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1f4h0ug</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Nail Design Inspired by A Goofy Movie Characters</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4h0ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1f4iowz</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Obsessed with my nails 🥹🫶🏽</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4iowz</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1f4f7ls</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Redo: Which nail shape looks better? Or which should I get?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4f7ls</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1f4g9a8</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Can I put a fake nail on top, or an extension/shellac/biab?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcaltxvbpold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1f4k3os</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>I just want to say….. THANK YOU to this sub for recommending the brush on nail glue from Kiss😍</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f4k3os/i_just_want_to_say_thank_you_to_this_sub_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1f4k0kh</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>First time I did nails</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4k0kh</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1f4jrv9</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fill in over colored acrylic </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f4jrv9/fill_in_over_colored_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1f4jffz</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frosted lavender candy nails! </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4jffz</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1f4j95e</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>my favorite color and I made them myself</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4al89n1fpld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1f4iwoa</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>No nail polish at new job</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f4iwoa/no_nail_polish_at_new_job/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1f4ii2h</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>First time using half tips with Polygel.</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4ii2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1f4i8fz</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Can this be fixed? There’s a line inside my nail bed.. then when it grows out it cracks in half. #NailTrauma</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7o7yl366pld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1f4hu8o</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m obsessed with Halloween sugar cookies 🎃 </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtwtxsgp2pld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1f4hrt0</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Birthday nails 🥳</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4hrt0</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1f4hgm3</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frog and Toad approved </t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frf19cpfzold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1f4gz0q</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>New day new look</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0oirmn2vold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1f4grv7</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>The retention on my coworkers nails 🤩🤩</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rezjycaktold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1f4gmgv</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s the most appropriate mani for a job interview? </t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f4gmgv/whats_the_most_appropriate_mani_for_a_job/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1f4gevc</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How would you recreate this look/color? </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4gevc</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1f4g38b</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Labor Day Set first piece</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4g38b</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1f4fqw1</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mixing gels </t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f4fqw1/mixing_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1f4fie9</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Feeling Catty 🐆💕</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0z1hjnmhjold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1f4few8</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Something blue 💙</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtmynwzpiold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1f4eawt</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>...</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4eawt</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1f4eik1</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>August nails</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyp6gbarbold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1f4eb58</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I'm in love with this style😍</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jr2n23y9old1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1f4e3xf</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>what do you think for this color?!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjciewzi8old1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1f4dwcm</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Almond nails are so classy </t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6t2bm6n07old1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1f4di3z</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>my first time at this salon and getting extensive nail art!! I LOVE THEM😍💖💖</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwxlhp204old1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1f4cqrc</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you use dual form stickers as airbrush/airbrushing stencils?  </t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95qm892eynld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1f4bqws</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Yellow french 🍋</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8433ccv4rnld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1f49ged</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Water tide inspired nails</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13ic7yn3anld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1f49gp3</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Inspired by my favorite puzzle!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f49gp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1f4b0an</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Lovful Press on</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4b0an</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1f4axjg</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>TIL About Chrome Powder</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4axjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1f4ap7x</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkly cat eyes 😻 </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1dzta6w7jnld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1f4af7s</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>First time doing Russian manicure🖤🤍🥀</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwf2nf08hnld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1f4a8yn</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>What color nail polish would look best with these colors?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jelmnmoxfnld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1f4a5oy</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>changed nail artist so i could have weapons lol</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4a5oy</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1f46gkt</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Pinching feeling at nailbed</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f46gkt/pinching_feeling_at_nailbed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1f499v8</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Delicate?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3ia9xot8nld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1f496fy</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching my current read </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pf4ikpf48nld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1f48ffs</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Possibly the cleanest DIY gel I’ve done ✨</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f48ffs</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1f48fm1</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Lifting</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f48fm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1f48ais</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">back to school nails 🤍 french tips always do the job </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qw9km12q1nld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1f471xg</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Help me find this color! Credit IG @jujhavens</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx2jo07rsmld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1f472ar</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Mosaic tile nails?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f472ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1f4805x</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>If my personality were nails:</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7tdfn0nzmld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1f47sxc</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>I started growing my nails out and painting them in May, it's now an obsession</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f47sxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1f47c68</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>The new press on nails are beautiful but now I can’t type😭</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxi3grotumld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1f4741b</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Aurora chrome nails- made by me</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihxnbpk6tmld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1f46zv8</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Love a thermal with a sparkly top coat 🥴</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f46zv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1f46zj5</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My girl rocked this set </t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyd88qj9smld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1f46xdt</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on Glue for reusable nails? </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f46xdt/press_on_glue_for_reusable_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1f46qx6</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>How can I improve my nails?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f46qx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1f46cki</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Chrome layer separating?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz9dbc2pnmld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1f45ofj</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which shape fits me best? </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f45ofj</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1f45acn</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>gel extensions I did today :)</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f45acn</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1f452dj</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t xml:space="preserve">showing off my last mani, in honor to the end of cold season </t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gawhypy8emld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1f44t8p</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>refreshing morning abundance. ✨</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svidhohfcmld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1f401vf</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>How long do you go between appointments?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f401vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1f43iup</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>What do I Book?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjnr42ux2mld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1f449mq</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>What do we think? I’m kind of obsessed 🥰</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f449mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1f447fx</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Did Opi nail envy dry out my nails?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njdg9xb18mld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1f446mb</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Which shape suits my hand best ?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f446mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1f43sz0</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Should I have my clients wear UV gloves?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f43sz0/should_i_have_my_clients_wear_uv_gloves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1f439tq</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>In love with the ilnp overcast collection🥹😍</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f439tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1f42orl</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried doing natural looking lesser claws </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oev6jj9mwlld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1f42obp</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Lasted 3 days but worth it lol</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/su1471oiwlld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1f42m9k</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Color suggestion for pedi</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f42m9k/color_suggestion_for_pedi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1f42jxn</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pretty in pink </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w65h38njvlld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1f427ti</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Big job interview today. Are these professional?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f427ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1f41tiv</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>watermelon set</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f41tiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1f41rl4</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Need to cut my natural nails off for my job</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnnaxxrfplld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1f413fc</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had to remove some gel polish because it lifted (despite doing appropriate cuticle and nail work) any advice to take care of nails? </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0luk34ijlld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1f40f8a</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">y’all loved my last set so this in the new and improved! 🩰 color is DND ‘sheer in the city’ (882) </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f40f8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1f40ddl</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail lady ate this - soft purples for end of summer </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f40ddl</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1f40ajd</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>How to keep nails from popping off?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f40ajd</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1f408ay</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Vampy 🎃</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06sa9vzfblld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1f405y1</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>After 3 months my natural nails</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46corgwtalld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1f3zppq</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t feel like this nail shape suits me </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bp1fnvb66lld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1f4pvem</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does hema free gel polish lessen risk of gel allergies? </t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4pvem/does_hema_free_gel_polish_lessen_risk_of_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1f4pqhs</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Matching my watch today 💙</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4pqhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1f4phrg</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Pearlescent Ivory Recommendations?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yk464l7f9rld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1f4pcxz</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Does bottle shape ever dictate your purchasing choices?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4pcxz/does_bottle_shape_ever_dictate_your_purchasing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1f4p7an</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Foggy tips of nails</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4p7an</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1f4od8w</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Forgot how much fun a topper over a simple creme is!!</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4od8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1f4nl1w</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s the prettiest nail polish you own? </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4nl1w/whats_the_prettiest_nail_polish_you_own/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1f4msj4</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Circe colors Rothko red ❤️</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4msj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1f4mdbg</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>My nails this past week 💅🏽</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4mdbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1f4lmhi</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wear it Purple Day: extra squishy edition </t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4lmhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1f4l0j7</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Millennium Mocha</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4l0j7</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1f4kyj3</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I never thought I would like a frosted metal this much </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6m07b1psupld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1f4kx3s</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4kolc</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1f4kb05</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Shoutout to my 'Fae Gatewarden for the Court of Dusk' ttrpg character. It's a fresh mess.</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dk7yy7popld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1f4k6is</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Current affairs is just gorgeous</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4k6is/current_affairs_is_just_gorgeous/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1f4jl65</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Nirvana</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4jl65</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1f4jble</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Hypnotized by my nails</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4jble</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1f4j4zl</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Conside me influenced. BKL lemon 🍋 </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4j4zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1f4imbf</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Joie de Vivre</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/blm36ioj9pld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1f4i8fx</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So hard to capture blue shimmer on pink nails </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4i8fx</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1f4hmpx</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Took a pic before I take these off and find some new colors. </t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xhc604v0pld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1f4hiwz</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Yeah, this sparks joy 💚</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4hiwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1f4hc5u</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pout Trout (lol) from Butter London idk about the name but is this a dupe for Gucci Peggy Sunburn or does that have more orange? Also can someone tell me how the formula is for the Gucci colors? </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4hc5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1f4guq9</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>First time doing my own gel nails and I love them</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4guq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1f4gd8j</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Mocha Cloud 👍</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4gd8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1f4g3g0</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY dupe - How’d I do? </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4g3g0</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1f4enwm</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">anybody got a Cirque lucky bag yet this August? </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4enwm/anybody_got_a_cirque_lucky_bag_yet_this_august/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1f4ensz</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Midtone cool green w/ pink/purple reflect?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4ensz/midtone_cool_green_w_pinkpurple_reflect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1f4d9gp</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last summer mani of the year </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q98gkaa72old1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1f4d32p</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I keep getting distracted by just how BRIGHT my fingers are </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk0t1dpv0old1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1f4ct96</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Essie Gel Top Coats</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4ct96/essie_gel_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1f4cpus</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bees knees Tree Sentinel </t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4cpus</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1f4cnhl</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Big Loud Lacquer moving sale</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4cnhl/big_loud_lacquer_moving_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1f4clkj</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>ILNP Olivia</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g6pl61hbtnld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1f4chgu</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>How long should you wait to paint your nails after having wet nails?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4chgu/how_long_should_you_wait_to_paint_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1f4cblo</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>You had me at HALO 😇 🩵</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4cblo</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1f4bb0i</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>A fun combo</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4bb0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1f4b3ri</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Regular lacquer over dip powder?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4b3ri</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1f4a0ao</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Bought 3 OG formula Nail Envy from Ebay seller but 2 don't have formaldehyde resin :(</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4a0ao</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1f49e9q</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really glad I saw these before they were all gone </t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8mg8tpo9nld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1f48sth</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>does anyone know the color name?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f48sth</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1f48olc</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Dollar Tree haul</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1axdha5j4nld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1f46adt</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Brittle nails</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f46adt/brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1f468hr</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Went down to the ol' harmacy and got some new lacquer!</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f468hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1f45vbw</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>KBShimmer Mystery~</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jhqwsw27kmld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1f45em5</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Lurid is gorgeous!</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f45em5</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1f450r3</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Toranja Jelly for my Birthday nails! </t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f450r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1f44c6g</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is a reasonable expectation for how long my polish will last? </t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f44c6g/what_is_a_reasonable_expectation_for_how_long_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1f436nh</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>What is the purpose of a peely base?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f436nh/what_is_the_purpose_of_a_peely_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1f42s0n</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Merkitten. Mooncat top coat. </t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f42s0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1f42gdj</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>🎄OPI Terribly Nice (Holiday Collection 2023) 🎄 Name your fave shade/s!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>/r/OPINailLacquerAddicts/comments/1f42e3a/opi_terribly_nice_holiday_collection_2023_name/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1f4161i</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first black holo! </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9ihqrr6klld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1f40i9r</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>bitchin’ by cirque colors - I am obsessed💜</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcbazne4elld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1f40fqo</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Onycholysis</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f40fqo/onycholysis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1f3zt0m</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Covering chips plus poor impulse control </t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3zt0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1f4p34q</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>diy french nails</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1j8dyri44rld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1f4p2g1</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>diy mettalic look nails</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wuf85qtp3rld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1f4lz9m</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Been trying to learn how to make my own press ons, and I really like how this set turned out!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8r8igjr4qld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1f4ljg8</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Just finished this one!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4ljg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1f4kwt8</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">#nail#vsalonnail #glittering nails#diy </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n19rma26upld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1f4kesr</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m a beginner and these are the first 3 nails I’ve ever done </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4kesr</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1f4jh1y</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frosted lavender candy nails! </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4jh1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1f4iipk</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>First time using half tips with Polygel.</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4iipk</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1f4humv</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I go crazy for the Halloween sugar cookies 🎃 </t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qeokm30t2pld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1f4ehh1</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>summer 😍😌[OC]</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hug6qng9bold1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1f4bnck</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>🌊</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4bnck</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1f4auix</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Isolated chrome attempt</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4auix</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1f48wse</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Summer colours</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8r9zwg76nld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1f43x9f</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Late Summer florals </t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f43x9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1f41ubu</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Watermelon set</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f41ubu</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1f3ypro</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Cats!</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f3ypro</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1f3xyyo</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>What gel nail polish brands do korean nail places use?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f3xyyo/what_gel_nail_polish_brands_do_korean_nail_places/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1f3xj8t</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adding them sparkles in life~ </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu3vmsy3gkld1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Aug 31 08:08:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_01.xlsx
+++ b/data/2024_09_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C976"/>
+  <dimension ref="A1:C1163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17028,6 +17028,3185 @@
         </is>
       </c>
     </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1f5hzeg</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would you do french, or white pedicure with these red colored Gaoy nails? </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vay2xgnfyld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1f5ho4l</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried red nails. </t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90i6qfmkbyld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1f5g406</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Over scrapped nails</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9ygbihfsxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1f56gkn</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Advice for getting better lines and shaping ?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f56gkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1f53agr</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Couldn't find a design I like so I made one up myself 🍻 </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gscn58lhnuld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1f51dv6</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Putting something on top of my nails to make them stronger?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f51dv6/putting_something_on_top_of_my_nails_to_make_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1f5h4z4</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Planning to get acrylic nails for the first time </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5h4z4/planning_to_get_acrylic_nails_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1f5ghaj</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Made some press-on nails for an anime🧡</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5ghaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1f5gh4f</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Baby pink French tips</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5gh4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1f5gf3s</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Flash/reflective polish</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5gf3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1f5g72a</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Old hands young nails </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5g72a</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1f5g0bf</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>did a set of pressons for myself!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m8ahnj8rxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1f5fyd8</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these bad? Be honest </t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83pabtdmqxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1f5fpqj</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Stray Kids Nails Part 2</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ebi6uyunxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1f5fejv</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to gift press on nails? </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5fejv/how_to_gift_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1f5f9xv</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails I just did. </t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3ss4qxyixld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1f5exg0</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Holo with some checkers!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyhgxci2fxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1f5ex36</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Perfect mirror effect </t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qsauqcyexld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1f5e8wa</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Sustainability when buying nails?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5e8wa/sustainability_when_buying_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1f5e501</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Is Ersanails legit</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5e501/is_ersanails_legit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1f5e2p4</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">are french tips supposed to look like this? </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5e2p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1f5dxw3</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Engagement nails 🥰</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ke3wkmw4xld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1f5dt1b</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Hearts and Promises | I Can Cer-Vive</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5dt1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1f5cuog</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">should i ask for a refund? </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x9x86y1uwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1f5ctch</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Press on or nail polish 💅</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5ctch/press_on_or_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1f5cfsa</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Finally getting a hang of polygel</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3zxfxz0qwld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1f5cep1</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails are stronger and growing more than ever lately, are these healthy? </t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6wpb12rpwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1f5bzwl</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>What Olive&amp;June nail polish is similar to OPI Big Apple Red? I really want to try something from O&amp;J but this is the only red I really like. Attached is an image of the color I’m trying to match.</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oltuibrlwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1f5bqde</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Trying to manifest Fall with these</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5bqde</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1f5bqcd</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Is it too early? 🎃 👻 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heiudkrajwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1f5bk2c</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>A recent y2k set I did</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5bk2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1f5bgh2</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Are their any nail painting tutorials that treat you as if you just found out that you have hands?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5bgh2/are_their_any_nail_painting_tutorials_that_treat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1f5bagd</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Baby boomer perfec</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hr6k1pbafwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1f5aziu</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frog nails 🐸 🩷 </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkzc7gjkcwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1f5auof</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5auof</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1f5alkf</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Oxblood season 🤌🏼</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5alkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1f5ah3b</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should I do? </t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxj01cs48wld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1f5a6ep</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Is this Brat?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwqcdtri5wld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1f5a2iz</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>I'm no pro but this is bad right?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5a2iz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1f59tsg</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Removal of gel on toes</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f59tsg/removal_of_gel_on_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1f596cs</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Hand painted designs 🖤</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f596cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1f58m2q</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>I was told to post this here 😅</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmfulk68svld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1f57wbc</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second attempt @ gel nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rib4j9cmvld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1f57sud</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time (gel) DIY! Pretty proud of myself 😇 </t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u3vgfjolvld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1f56nt4</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winnie Pooh Nailart </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f56nt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1f56hpt</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Small nail beds mani</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jlvqgbgbvld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1f568f5</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Temperature changing nails!(Light pink when warm, maroon when cool.)</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f568f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1f55myx</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Wanted my nails to reflect my feelings of growth this summer 🦋</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f55myx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1f55b7n</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>What nail shape would suit my hands? I got almond last time but they look off. Just me?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f55b7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1f55b44</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thin press on nails? </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f55b44/thin_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1f54s1j</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you guys remember Bobby jack?? I love this set I did for my bestie </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f54s1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1f54l2h</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>first attempt at almond🫢</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yekcnkjdxuld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1f54eye</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Found my new favorite way to take nail pics </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f54eye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1f54cal</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>My nails for starting 10th grade 🙃</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bmx4qaivuld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1f5473p</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Short and Sweet</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5473p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1f53z0t</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Botched?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f53z0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1f53v27</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Hand painted Glass Animals press ons</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1dbovqtruld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1f53txp</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Why’d she file them so short?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8c67708nruld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1f53ntv</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>For the love of color🦕🦣</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sguv6qfaquld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1f53mub</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Made my first press on nails</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/us6nnuh4quld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1f53g0b</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>End of summer nails 🌤️</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f53g0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1f53026</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Neon pedi</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f53026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1f52xto</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>First time using acrylic paint in a design. Turned out better than I thought it would??</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f52xto</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1f52hs0</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What's going on with my thumb nail? </t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f52hs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1f52fme</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The best background for nails is a cat </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f52fme</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1f52b73</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>yay or nay? 🐠</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f52b73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1f5242a</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honeydew 🍈 </t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlqf8zuoeuld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1f51h15</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Football</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f51h15/football/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1f51eyw</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Retaining nail length?</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f51eyw/retaining_nail_length/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1f50jvs</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday set 🌞 </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xiemyr533uld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1f4m7zy</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Practice does make perfect! Don't give up!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4m7zy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1f4pk00</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>gojo nails 🙂‍↕️🙂‍↕️🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4pk00</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1f4sivc</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Had to cut down my nails and I'm devastated</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4sivc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1f4tteo</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obb15je2nsld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1f50eym</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Technician left on gel-x before hard gel? Is that normal?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f50eym/technician_left_on_gelx_before_hard_gel_is_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1f50ewo</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What colour should I try on nails? </t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f50ewo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1f50drq</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>End of summer nails!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1t6utwv1uld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1f500g2</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>All the designs/colors I’ve ever gotten since I started getting acrylics, What should I do next?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnx487y5ztld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1f4zru1</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Can I use regular polish over biab?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1oqnb8extld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1f4zijw</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>My nail journey!</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4zijw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1f4z6fh</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t xml:space="preserve">two days growth. is this normal ?? </t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hiuik6kwstld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1f4z5uy</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Essie Fairy tailor</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9h3mjmsstld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1f4z1th</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>what shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4z1th</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1f4ycnf</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 Tone Cow Print 🐮 ♥️ </t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6i0325smtld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1f4yar4</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Last of the summer nails, before the fall &amp; holidays sets 🤩</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ri6u5idmtld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1f4y78g</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Nails for Wedding</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lel6y22mltld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1f4lli8</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>my nails are very damaged after taking off press ons, what do i do now?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4lli8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1f4y2mj</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>How long does it take for your nails to grow?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4y2mj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1f4xv7c</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are they supposed to clean the cuticles and skin around the nails? I feel like this wasn’t a great quality manicure. Really I was mostly hoping for the skin to be cleaned up. So I have to ask for something specific? </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4xv7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1f4xbaq</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>New aura design, i'm in love</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fjwber7ftld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1f4wwn3</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are at home dip powders like Sassy Saints healthy for your nails? </t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f4wwn3/are_at_home_dip_powders_like_sassy_saints_healthy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1f4wssq</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help w/ damaged nails </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4wssq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1f4wafh</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Flowery nail art</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mt7tlmrh7tld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1f4w4x9</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Can do better</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4w4x9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1f4vqtx</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic overlay and gel polish I did myself </t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4vqtx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1f4ut21</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this cuticle? It’s hard to get off </t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zj84ntrpvsld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1f4uhui</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Nails breaking</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epjvueh2tsld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1f4ufht</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally got a set worth posting here </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvkrgtpissld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1f4u6zc</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do these look too mucho like falsies?? </t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4u6zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1f4u6fo</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So, I tried something different </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4u6fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1f5gzlc</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Over buffed nails</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f5gzlc/over_buffed_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1f5grp6</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>My nails look bulbous</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5grp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1f5ftsx</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>💿🩱riding waves🩱💿</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3gezjw5pxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1f5fiy2</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>💗✨my kink is watching you ruin your life✨💗</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vejnil0tlxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1f5fgmd</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail lady ruined my nails </t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5fgmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1f5e7ob</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I like red </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/si8a40tn7xld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1f5e4wm</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Please help me find this persons shade!! they wpnt reply (its gel)</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bnp8qnw8sld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1f5dv79</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>not to be dramatic or anything, but doing my nails changed my life</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5dv79</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1f5drqo</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Hearts and Promises | I Can Cer-Vive</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5drqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1f59bxq</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Indie Brand Comparison</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f59bxq/indie_brand_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1f5cqow</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>I’m not ready for summer to be over 😭</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5cqow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1f5cjvr</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Labor Day Sales</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f5cjvr/labor_day_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1f5cgml</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>72 full hours of wear without a single chip</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5cgml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1f5ce3v</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>I get it now</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olbj08umpwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1f5bwz8</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Shleee Polish Soul</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fb7qeljykwld1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1f5brh9</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">made press-ons for my vacation!! </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hcxhmmljwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1f5at62</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Y’all didn’t tell me ILNP’s packaging was so cute?!</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rr6aqk2bwld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1f5a8pv</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Dr. Pepper Nails</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6ybfnl36wld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1f58oyh</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Salon drilled off my proximal fold 2 months ago?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qewhwcwwsvld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1f58374</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Perhaps the most beautiful polish I’ve ever seen!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f58374</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1f576ns</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Spooky szn is upon us 👻🎃</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f576ns</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1f56pd5</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own tips n gel for the first time, tried to go for a porcelain vibe </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f56pd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1f56kga</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Berry-toned jelly nails </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f56kga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1f56ddl</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Temperature changing nails! (Light pink when warm, maroon when cool.)</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f56ddl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1f56b7q</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL Lemon 🍋 </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f56b7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1f56789</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>QUICK SOS</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uz81jzw99vld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1f55ue4</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Forces of Evil </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f55ue4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1f55aaf</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Mega </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymgij1rf2vld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1f559p5</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Glisten and Glow favorites?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f559p5/glisten_and_glow_favorites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1f55515</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>The shadow is cracking me up</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezh0pu3f1vld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1f551fs</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Back to basics (kinda)</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f551fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1f54sgw</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>venom by ilnp</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f54sgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1f54pua</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lurid Lacquer Halloween Countdown Calendar </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f54pua/lurid_lacquer_halloween_countdown_calendar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1f5411a</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkles and stamps </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5411a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1f53u24</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Can someone tell me why this happens with seche vite top coat?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f53u24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1f53sot</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupes? (excluding cirque color's moonstone) </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f53sot/dupes_excluding_cirque_colors_moonstone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1f537nh</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What the heck happened Fancy Gloss?? </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f537nh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1f521nu</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Very demure, very mindful 🎀</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f521nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1f51ymt</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Starting Off Fall Strong</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqfu8yjjduld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1f51vwu</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Lyn B Trouvaillle ✨</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f51vwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1f51g8w</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>I know my nails are too long when my partner says "OMG look at those witchy talons!!"</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f51g8w/i_know_my_nails_are_too_long_when_my_partner_says/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1f51bth</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Finally tried Reddish Purple Pencil (with real pencil shavings) from Death Valley Nails and my feelings are…mixed</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f51bth</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1f519p1</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>I love it when the newbies go together</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zjs3qag8uld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1f5186n</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Any dupes for my beloved (but discontinued) Lapiz of Luxury by ESSIE?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8yt1jyx48uld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1f50m5f</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>My nails are blushing! LA Colors Sheer Jelly</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zf7n6jad3uld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1f50jpv</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>My first Cupcake Polish: Lord licorice</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vx8sp7y23uld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1f4zxek</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Fairy Tailor </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwzp3l7kytld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1f4zs2r</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tom Cruise is one of those people who might ask weird questions about long nails like discussed in a recent post.  </t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://twitter.com/filmupdates/status/1828869477741801666?s=46</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1f4yejj</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>I might be a teal/turquoise lover now</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4yejj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1f4xlys</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>I Forgive You ✨</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4xlys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1f4xfpq</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>What are your biggest tips to keep your cuticles soft and help prevent compulsive skin picking?</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4xfpq/what_are_your_biggest_tips_to_keep_your_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1f4x4wc</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Found an elegant and pretty combo!</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4x4wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1f4wrfy</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Essie Gel Couture in Take me to Thread</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tamur02btld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1f4weso</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Fall Combos with Bottled Rage</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4weso</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1f4wer2</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Any Crème Recs?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8l1ubje8tld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1f4wc8g</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>I am in Spain without the 'S'</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4wc8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1f4ve74</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>For those who wanted to see swatches</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4ve74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1f4v712</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Third try with polygel, complete nail beginner </t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lnqh97yysld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1f4t9mt</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Tried a drag marble for the first time!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4t9mt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1f4t6h4</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Struggling to find a method that works out of gel/normal/falsies/dip/wraps. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f4t6h4/struggling_to_find_a_method_that_works_out_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1f4sxq4</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Not very pretty, but still cool ✨</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yigg7g0nesld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1f4rrf2</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Such a glowy nail polish! </t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4rrf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1f4rpp6</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>My shorty manis in August</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4rpp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1f5i2c8</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>I’m dying to know how to recreate these gorgeous nails</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5i2c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1f5hll1</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newbie to nail art </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emuu4n9nayld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1f5g1qx</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Valentines nails from ages ago 🩷❤️🤍</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0jy5uqorxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1f5fsld</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes you just have to make a mini frog 🐸 </t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a06pmz9soxld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1f5f67e</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Finding Nemo nails</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5f67e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1f5c21q</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newest set </t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5c21q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1f5a8aq</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling fall. Loving the copper chrome! </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g857hgpz5wld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1f59bev</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Finally attempted the pool water trend! 💦🌸</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f59bev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1f598md</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Reflective butterfly wings🦋✨</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f598md</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1f58j6s</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Some frogs for you 😀</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ek8q9tjkrvld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1f58f3u</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help understanding this design </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc8h3mtnqvld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1f57lqg</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Funky set 🩷⭐️🖤</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f57lqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1f55q6q</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Which ones should I get?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f55q6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1f52yiv</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Neon pedi</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f52yiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1f4zvvl</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Toddler with an eye for color</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofqd4cv8ytld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1f4zpd5</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>which ones are prettier?</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4zpd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1f4yiun</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>My first set. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krb3i0y2otld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1f4x3v9</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Thanks Jazz from LA. I really love it!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0k2nhp9ldtld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1f4wj3t</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>new in nailart stuff, i keep messing up</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f4wj3t/new_in_nailart_stuff_i_keep_messing_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1f4wdlk</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spontaneous flowers </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4wdlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1f4v58p</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beautiful french style nails😌[OC]</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxpohmubysld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1f4ur4w</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>90s grunge nails for the Pearl Jam concert!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lq04fs9vsld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1f4u5ka</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>The pandemic DIY nail art ~</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqzez2e4qsld1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1f4jm8z</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Which is better, pink or blue?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f4jm8z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Sep  1 08:09:07 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_09_01.xlsx
+++ b/data/2024_09_01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1163"/>
+  <dimension ref="A1:C1329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20207,6 +20207,2828 @@
         </is>
       </c>
     </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1f68pdx</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>my recent nails</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ti3gusgf5md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1f68otp</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Working on a set of press ons for my wedding, opinions and advice welcome. </t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f68otp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1f66hiw</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Does anyone know why this happens after a manicurist trims my cuticles? (Forgive the jagged nail)</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1gkx3jzo4md1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1f67ljd</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My cat eye comic book nails ❤️ </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tva4z4cx15md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1f66j2b</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Three weeks apart </t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f66j2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1f66cin</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Can you guys help me figure out which nail shape suits my hands</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppez1hugn4md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1f65xn1</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Are these nicely done?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f65xn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1f659ax</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">when to use builder gel? </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f659ax/when_to_use_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1f64hrk</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Nails &amp; things! 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f64hrk/nails_things/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1f6486m</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Cinderella Blue🩵 Polygel Overlay✨</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dtjfvfrp14md1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1f6420c</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting spooky season early. </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sq8xluv304md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1f63ywm</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>new set</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ar92l178z3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1f63tjk</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Ombré </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9gg95jsx3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1f63lm1</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Autumn Pumpkin Spice Nails</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f63lm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1f633gz</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vampire vibes 🧛‍♀️ </t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qaaflxrq3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1f62unz</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>First time getting soft gel! They change color depending on lighting and angles COOL</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f62unz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1f629lq</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Hubby painted my nails for me ❤️</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6zhyw7vi3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1f620dc</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fine art kitties 🐱 </t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nbi6p1gg3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1f61v6o</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pre fall nails 🍁 </t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p21qfvx3f3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1f612dj</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Super cute Frog 🐸</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l25p9ydv73md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1f60tdf</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rubber base PSA </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lb1b9tsn53md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1f60n4h</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Nailpatella Syndrome ManicureTips?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f60n4h/nailpatella_syndrome_manicuretips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1f60iwc</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>My nail tech does not play!!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f60iwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1f60i33</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>I did my friend's nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmymevnx23md1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1f60c1m</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Is the ripple (?) /uneven surface of my polish the shape of my nail or the polish itself?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f60c1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1f607jz</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte short stiletto nails, new fave </t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f607jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1f6065g</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>New set 🥰</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o37b2d4403md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1f605bd</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's just that the wine color is simply beautiful and elegant. </t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f605bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1f6052o</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Cute ombre french manicure</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ywpt5muz2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1f5zw4e</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Finding a good nude color is so satisfying</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhuekcwqx2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1f5yibq</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Do you think the stones I used were way too big?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5yibq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1f5yq5h</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>French love bow decor nails</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bwhkwnln2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1f5yotp</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>worth it 😯</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gxo5cben2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1f5yhiq</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How did this turn out ? </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5yhiq/how_did_this_turn_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1f5ygom</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Please look at this beauty</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/noasg9hil2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1f5ydr9</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Went with this design in the end</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tktskqjtk2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1f5yays</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Been in a bit of a nude phase</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5yays</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1f5xqto</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Apres gel x dupes??</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5xqto/apres_gel_x_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1f5xhzk</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Just call me the Michael Bay of Nails</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5xhzk/just_call_me_the_michael_bay_of_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1f5xfz9</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Decided to do something different today</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5xfz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1f5xeg9</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Tried press ons for the first time since I was 13</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gxq7v2tc2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1f5x5zh</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>What do we think of this?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71piccz0b2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1f5x3k0</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Press ons by moi ☺️</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5x3k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1f5wwjg</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">vacay nails </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flmj40b092md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1f5wrgj</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Can I save old nail polish?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5wrgj/can_i_save_old_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1f5wat5</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suggestions for nude pink polish </t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1l4xz04642md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1f5t8v3</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Which set should I wear?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5t8v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1f5u649</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Broke my nail down to the skin, what do I ask my stylist to do?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kpcey46n1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1f5w8ii</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>What colors am I missing?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkee9c1o32md1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1f5vmk7</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel extension/fake nails </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5vmk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1f5w7j1</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>My natural nails with classic nail polish</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqw0esxf32md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1f5w1lp</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Sunflower season 🌻</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ox7cojd522md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1f5vy2x</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Just simple</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63612yzb12md1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1f5vsau</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>simple builder mani!</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/188v9tr002md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1f5vrx2</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glazed trend </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5vrx2/glazed_trend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1f5v530</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>My Cartagena nails 🖤</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35o7ox6wu1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1f5v1dx</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally getting the French down </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm6dfju2u1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1f5udpf</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Steampunk Fever Dream</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5udpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1f5trly</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>my husband called these “sailor moon nails” 😂🌌</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfr9xu7zj1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1f5thsy</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Real Flowers </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ahv8ghvh1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1f5t8r6</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">this might be the prettiest set of press ons I’ve ever had 🍑 </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrbil5fvf1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1f5t1nr</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>This post-anxiety guy needs your help...</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5t1nr/this_postanxiety_guy_needs_your_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1f5sxyg</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for September! </t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mi5tgqvhd1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1f5rzhh</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>I love red nails</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5rzhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1f5rlie</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Bare nails ready for Culinary School!</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0giij8t031md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1f5rd7c</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>wine red nails 🍷❤️</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dc8751711md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1f5r0dj</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>New nails! What do you think about that color?</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxd2vmkfy0md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1f5qv81</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Just a little yellow..</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqvxp8r9x0md1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1f5qlpn</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>First set of acrylic nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sphviaz8v0md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1f5pogj</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Mother of Pearl Nails</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vrhhr71o0md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1f5p9sg</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">YEEHAW! </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5p9sg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1f5oxdw</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Would it be rude at the nail salon if I brought a press-on nail to show the nail tech the shape I want?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5oxdw/would_it_be_rude_at_the_nail_salon_if_i_brought_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1f5okox</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>It is time for Halloween colors 🎃</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnz1tql9f0md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1f5oa6q</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons! </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p94b17wtc0md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1f5nkoe</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Deadpool nails</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5nkoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1f5lzyj</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Is 32 Eur too expensive for this bottle of soft gel?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f0iqi7hszld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1f5lrnf</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>💀😎</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko1xy3n6qzld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1f5lf4v</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Back to school 🍎🍏</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u1hnclkmzld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1f5lck3</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to clean up scuff marks? </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5lck3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1f5l3aa</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Dark glittery fuchsia ✨</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcjpgqqxizld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1f5l16e</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>I see you 🧿</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5l16e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1f5k48p</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>it's really shitty, but it was for a reunion with my best friend after a month, I had to have my nails done (trying square for the first time)</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5k48p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1f5k0t1</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Not sure the best shape for my nails?!</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5k0t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1f5jsuo</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>I like the tortoise. Not sure if gold suits my skin tone…</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5jsuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1f5igac</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Looking to start doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f5igac/looking_to_start_doing_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1f68i8v</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>help finding clear polish!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f68i8v/help_finding_clear_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1f66vab</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Velvet effect topcoat help </t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f66vab/velvet_effect_topcoat_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1f66jy3</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>How to: Chrome powders on regular nail</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n59myzypp4md1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1f66b37</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Glisten and Glow polishes feedback</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f66b37/glisten_and_glow_polishes_feedback/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1f65ahs</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>What in the world</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qfzs8fcc4md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1f6561t</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Looking for thoughts on the Holo Taco nail oil pen</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f6561t/looking_for_thoughts_on_the_holo_taco_nail_oil_pen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1f64vbd</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>When it comes to beautiful nails...</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/es1a2og684md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1f64e42</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>amethyst dart frog 🔮🐸</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edd4s09d34md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1f646kk</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Overcast skittle ☔️ </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f646kk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1f6341q</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Wasn’t sure I was feeling pink today but I’m sold now 😍</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8gwnbjxq3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1f62wi0</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>What are your top 5 brands?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f62wi0/what_are_your_top_5_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1f62kvh</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Loving this purple and blue skittle</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f62kvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1f621vb</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Cirque Colors: Mxcn Cola Jelly</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tfwk0eug3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1f61qxn</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>an ORLY Bonder hate post</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f61qxn/an_orly_bonder_hate_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1f616of</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DND polish help question </t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f616of/dnd_polish_help_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1f60zkg</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Week old mani</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f60zkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1f60pzg</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Time Painter, Sally Hansen + NailTek Nail Recovery </t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f60pzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1f60b9d</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Vanishing polish?!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7w38ur6a13md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1f6032p</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Trying to grow my natural nails back out!</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58skmcddz2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1f5zu28</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Tried Death Valley Nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjzvoca9x2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1f5zneb</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Current Obsession — Essie’s Sheer Fantasy 🎀</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5zneb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1f5zgd4</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vertical cracks in polish </t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/in8t04qtt2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1f5zec0</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cock A Doodle Doom's sparkling sisters </t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6894lbaft2md1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1f5zdro</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Rant on skin-color creams</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5zdro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1f5z8p2</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>I was going for checkerboard cookies did it work</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tk4dbrlsr2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1f5yukl</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Ethereal blobs</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5yukl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1f5ypax</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Paris Olympics Color Scheme Nails</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5ypax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1f5ykzl</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Forces of Evil</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5ykzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1f5ybr0</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>FYI for nail staining</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07qzdb3dk2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1f5y128</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Subtle Palette Cleanser</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5y128</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1f5xl9m</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Long time lurker, first time poster</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5xl9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1f5x089</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Flaky fun</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5x089</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1f5w4so</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very fun green </t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5w4so</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1f5viyu</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Help! Terrible staining</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5viyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1f5va76</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Last mani of the summer</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aay0gkrzv1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1f5v8cm</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>People with Helmers: do the drawers squeak?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7i0upslv1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1f5v73k</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Not Tonight</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5v73k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1f5v728</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Comparison photos from when I first started my journey of stopping picking/biting my nails, vs now (same polish)</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5v728</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1f5uc14</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Thermals make me want to grow out my nails</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5uc14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1f5u2e3</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Neon pink swatch comparison</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yy7fedycm1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1f5trfo</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to recreate purple jellie shoes from my childhood </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9cjoejsj1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1f5tmdd</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Y2Slay + bonus</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5tjnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1f5tl5r</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t xml:space="preserve">glazed donut nails! so smooth and perfect 😍 by me! (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9xf3fjmi1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1f5t8l9</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>I love Pahlish’s Chappell Roan-inspired polishes! 💓</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5t8l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1f5sxsb</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How Do I make my nails not look so terrible </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pf5p46zfd1md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1f5s2d6</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>I thought I ‘didn’t have many reds’ 😅😳</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc29dyim61md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1f5rksq</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">broken nail *temp* fix </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zg7whq6v21md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1f5rdr0</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>This weeks nails!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn1qwl3b11md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1f5r8bm</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>I wanted to mention Le Mini Macaron packaging! Cuuuute 💖</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5r8bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1f5r0c8</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Just a little yellow..</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjibrsiby0md1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1f5qtdj</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A very pretty TKMaxx Find. </t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5qtdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1f5qe5u</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>went to matchbox twenty last night...</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5qe5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1f5q83v</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using gel extensions from Le Mini Macaron!! Love them :) </t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5q83v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1f5pdtq</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Snow and Ashes ❄️🌋</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5pdtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1f5p226</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Boom 💣🔥</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j7q0k786j0md1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1f5o965</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Melody by ILNP unsure of this color on me</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvlg25j2c0md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1f5o61r</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to dupe baja blasted by layering. Still want it though </t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5o61r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1f5o36c</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>✨Glowstick?! More like Whoastick!✨</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tb12zke8b0md1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1f5nc6x</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Are Lurid Lacquer’s polishes always so thick?</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f5nc6x/are_lurid_lacquers_polishes_always_so_thick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1f5mw4z</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fix overgrown nail beds? </t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1mnhyzz00md1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1f5mtpv</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This polish confuses me </t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5mtpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1f5ms5u</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Nightcrawler by Mooncat Topped with Jinx by ILNP and Glossy Taco by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5ms5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1f5mb77</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stain on regular (non-gel) nail polish - how to remove? </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8s5r43kvzld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1f5m9ej</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Alright, you guys were right about ILNP’s Bluebell</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8aepjj2vzld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1f5lfb5</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Alien vs Pond</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1h7bg6bmmzld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1f5l711</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>The retiree and the new sheriff in town. Any tips how to keep the top coat from lifting the colour and getting ruined? I don't know if you can see in the pic but the Barry M one is pretty much pink 😬</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3726jks3kzld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1f5ikpf</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>All I want are long nail beds 🥲</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5ikpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1f63xae</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>ombre attempt</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8yaeh7psy3md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1f62uxv</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Stocking up on supplies</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f62uxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1f60p52</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Proud of my press ons</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f60p52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1f5yro5</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>3 hrs 🥴</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by8eka31o2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1f5yjjf</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Stones too big?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5yjjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1f5x2il</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Press ons by moi ☺️</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5x2il</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1f5x1rd</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Iridescent monarch nails</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2z63024a2md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1f5wlbd</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tropical nail trend 😍 </t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5wlbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1f5rkdz</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>are my nails pretty?[OC]</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7a05vaj21md1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1f5qxux</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Just a little yellow..</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ziricntux0md1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1f5p6k9</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Just call me the Michael Bay of Nails</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/52nqdo87k0md1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1f5mn60</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Biutifull </t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04ikkgmryzld1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1f5l9v7</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Cherries 🍒 Done by Eric at Get Nailed Salon in NYC :)</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5l9v7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1f5jv1j</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying some new nails </t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f5jv1j</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>